<commit_message>
added game consoles and tumble dryers
</commit_message>
<xml_diff>
--- a/data/consumption statistics/EnergyConsumption.xlsx
+++ b/data/consumption statistics/EnergyConsumption.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ComputersMoniors" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="Lighting" sheetId="5" r:id="rId3"/>
     <sheet name="TVs" sheetId="6" r:id="rId4"/>
     <sheet name="ElectricHeaters" sheetId="7" r:id="rId5"/>
+    <sheet name="GameConsoles" sheetId="8" r:id="rId6"/>
+    <sheet name="TumbleDryers" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="133">
   <si>
     <t>Uses/ hours</t>
   </si>
@@ -375,6 +377,48 @@
   </si>
   <si>
     <t>are more visually pleasing and take up less space as they are mounted on to the wall</t>
+  </si>
+  <si>
+    <t>Original PS3</t>
+  </si>
+  <si>
+    <t>PS3 Slim</t>
+  </si>
+  <si>
+    <t>Xbox 360</t>
+  </si>
+  <si>
+    <t>Xbox 360S</t>
+  </si>
+  <si>
+    <t>Nintendo Wii</t>
+  </si>
+  <si>
+    <t>Xbox One</t>
+  </si>
+  <si>
+    <t>PS4</t>
+  </si>
+  <si>
+    <t>Cycles per year</t>
+  </si>
+  <si>
+    <t>kW per use/ cycle</t>
+  </si>
+  <si>
+    <t>Load (kg)</t>
+  </si>
+  <si>
+    <t>Energy Efficiency</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -2452,8 +2496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2524,18 +2568,18 @@
         <v>1.2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D25" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D23" si="0">B3*C3</f>
         <v>1314</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E25" si="1">D3*0.17</f>
+        <f t="shared" ref="E3:E23" si="1">D3*0.17</f>
         <v>223.38000000000002</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G7" si="2">C3*100</f>
+        <f t="shared" ref="G3:G4" si="2">C3*100</f>
         <v>120</v>
       </c>
       <c r="H3" t="s">
@@ -2593,7 +2637,7 @@
         <v>20</v>
       </c>
       <c r="G5">
-        <f>C5*100</f>
+        <f t="shared" ref="G5:G18" si="3">C5*100</f>
         <v>200</v>
       </c>
       <c r="H5" t="s">
@@ -2622,7 +2666,7 @@
         <v>40</v>
       </c>
       <c r="G6">
-        <f>C6*100</f>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="H6" t="s">
@@ -2651,7 +2695,7 @@
         <v>100</v>
       </c>
       <c r="G7">
-        <f>C7*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="H7" t="s">
@@ -2680,7 +2724,7 @@
         <v>100</v>
       </c>
       <c r="G8">
-        <f>C8*100</f>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="H8" t="s">
@@ -2709,7 +2753,7 @@
         <v>100</v>
       </c>
       <c r="G9">
-        <f>C9*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="H9" t="s">
@@ -2738,7 +2782,7 @@
         <v>100</v>
       </c>
       <c r="G10">
-        <f>C10*100</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="H10" t="s">
@@ -2767,7 +2811,7 @@
         <v>120</v>
       </c>
       <c r="G11">
-        <f>C11*100</f>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="H11" t="s">
@@ -2796,7 +2840,7 @@
         <v>120</v>
       </c>
       <c r="G12">
-        <f>C12*100</f>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="H12" t="s">
@@ -2825,7 +2869,7 @@
         <v>30</v>
       </c>
       <c r="G13">
-        <f>C13*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="H13" t="s">
@@ -2854,7 +2898,7 @@
         <v>30</v>
       </c>
       <c r="G14">
-        <f>C14*100</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="H14" t="s">
@@ -2883,7 +2927,7 @@
         <v>50</v>
       </c>
       <c r="G15">
-        <f>C15*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="H15" t="s">
@@ -2912,7 +2956,7 @@
         <v>50</v>
       </c>
       <c r="G16">
-        <f>C16*100</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="H16" t="s">
@@ -2941,7 +2985,7 @@
         <v>50</v>
       </c>
       <c r="G17">
-        <f>C17*100</f>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="H17" t="s">
@@ -2970,7 +3014,7 @@
         <v>60</v>
       </c>
       <c r="G18">
-        <f>C18*100</f>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="H18" t="s">
@@ -2999,7 +3043,7 @@
         <v>40</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G23" si="3">C19*100</f>
+        <f t="shared" ref="G19:G23" si="4">C19*100</f>
         <v>40</v>
       </c>
       <c r="H19" t="s">
@@ -3028,7 +3072,7 @@
         <v>50</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="H20" t="s">
@@ -3057,7 +3101,7 @@
         <v>50</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="H21" t="s">
@@ -3086,7 +3130,7 @@
         <v>70</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="H22" t="s">
@@ -3115,11 +3159,347 @@
         <v>100</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="H23" t="s">
         <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>730</v>
+      </c>
+      <c r="C2">
+        <v>0.189</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>137.97</v>
+      </c>
+      <c r="E2">
+        <f>D2*0.17</f>
+        <v>23.454900000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>730</v>
+      </c>
+      <c r="C3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="0">B3*C3</f>
+        <v>62.050000000000004</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" si="1">D3*0.17</f>
+        <v>10.548500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>730</v>
+      </c>
+      <c r="C4">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>125.55999999999999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>21.345199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5">
+        <v>730</v>
+      </c>
+      <c r="C5">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>64.239999999999995</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>10.9208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6">
+        <v>730</v>
+      </c>
+      <c r="C6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>11.68</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>1.9856</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7">
+        <v>730</v>
+      </c>
+      <c r="C7">
+        <v>0.11</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>80.3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>13.651</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8">
+        <v>730</v>
+      </c>
+      <c r="C8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>102.2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>17.374000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>150</v>
+      </c>
+      <c r="B2">
+        <v>3.35</v>
+      </c>
+      <c r="C2">
+        <f>A2*B2</f>
+        <v>502.5</v>
+      </c>
+      <c r="D2">
+        <f>C2*0.17</f>
+        <v>85.425000000000011</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="B3">
+        <f>C3/A3</f>
+        <v>4.1568627450980387</v>
+      </c>
+      <c r="C3">
+        <f>D3/0.17</f>
+        <v>623.52941176470586</v>
+      </c>
+      <c r="D3">
+        <v>106</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>150</v>
+      </c>
+      <c r="B4">
+        <f>B5*B2/B3</f>
+        <v>3.2867924528301891</v>
+      </c>
+      <c r="C4">
+        <f>A4*B4</f>
+        <v>493.01886792452837</v>
+      </c>
+      <c r="D4">
+        <f>C4*0.17</f>
+        <v>83.813207547169824</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>150</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B4:B7" si="0">C5/A5</f>
+        <v>4.0784313725490193</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C4:C7" si="1">D5/0.17</f>
+        <v>611.76470588235293</v>
+      </c>
+      <c r="D5">
+        <v>104</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <f>B7*B4/B5</f>
+        <v>1.3589622641509433</v>
+      </c>
+      <c r="C6">
+        <f>A6*B6</f>
+        <v>203.84433962264151</v>
+      </c>
+      <c r="D6">
+        <f>C6*0.17</f>
+        <v>34.653537735849056</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1.6862745098039214</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>252.9411764705882</v>
+      </c>
+      <c r="D7">
+        <v>43</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>